<commit_message>
Implementando: getAsString, findByName e getElementAt.
</commit_message>
<xml_diff>
--- a/Aula02/MemóriaAlunoCurso-v2.xlsx
+++ b/Aula02/MemóriaAlunoCurso-v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="27">
   <si>
     <t>null</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>last</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>índice</t>
   </si>
 </sst>
 </file>
@@ -1983,6 +1989,56 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>183932</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>26275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>183931</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>13137</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Conector de Seta Reta 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3849415" y="4302672"/>
+          <a:ext cx="1832740" cy="755431"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2253,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25:L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2265,21 +2321,21 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="I4" s="5" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="I4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="M4" s="5" t="s">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="M4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
@@ -2354,29 +2410,29 @@
       <c r="O7" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="I11" s="5" t="s">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="I11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="M11" s="5" t="s">
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="M11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -2436,18 +2492,18 @@
       <c r="O14" s="4"/>
     </row>
     <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="I17" s="5" t="s">
+      <c r="F17" s="6"/>
+      <c r="I17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="M17" s="5" t="s">
+      <c r="J17" s="6"/>
+      <c r="M17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N17" s="5"/>
+      <c r="N17" s="6"/>
     </row>
     <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="2"/>
@@ -2497,29 +2553,52 @@
         <v>9</v>
       </c>
     </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>22</v>
       </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
       <c r="I24" t="s">
         <v>22</v>
       </c>
+      <c r="K24" t="s">
+        <v>26</v>
+      </c>
+      <c r="P24" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
       <c r="N25" t="s">
         <v>22</v>
       </c>
+      <c r="P25">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="E26" s="5" t="s">
+      <c r="C26" s="5"/>
+      <c r="E26" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
@@ -2589,14 +2668,14 @@
       <c r="C32" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="H32" s="5" t="s">
+      <c r="F32" s="6"/>
+      <c r="H32" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="5"/>
+      <c r="I32" s="6"/>
     </row>
     <row r="33" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E33" s="2"/>
@@ -2665,18 +2744,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="M11:O11"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="M11:O11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>